<commit_message>
Updating the research document and the testing documents
</commit_message>
<xml_diff>
--- a/Frontend & Backend Testing Documents/Testing Plan.xlsx
+++ b/Frontend & Backend Testing Documents/Testing Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5464169ef79c6a16/Desktop/Computing Years/Computing Year 4/Collaborative Project (Year Long)/Frontend ^0 Backend Testing Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5464169ef79c6a16/Desktop/Computing Years/Computing Year 4/Collaborative Project (Year Long)/PROJECT DOCUMENTS - GITHUB ^0 NEW/Frontend ^0 Backend Testing Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{197E27B6-EA79-42FA-A7D8-FC34330D7B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{197E27B6-EA79-42FA-A7D8-FC34330D7B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12FE6A98-E6E5-4309-8FF4-6AB7E6BCECCE}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{66ECC141-54E1-4219-8EEA-79F64E297CAC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{66ECC141-54E1-4219-8EEA-79F64E297CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend Test Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>TestID</t>
   </si>
@@ -57,21 +57,6 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>Create Account Button</t>
-  </si>
-  <si>
-    <t>Login Button</t>
-  </si>
-  <si>
-    <t>Logout Button</t>
-  </si>
-  <si>
-    <t>Scan Button</t>
-  </si>
-  <si>
-    <t>NavBar Burger Menu Icon</t>
   </si>
 </sst>
 </file>
@@ -301,40 +286,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -584,13 +535,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -624,6 +568,47 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -638,15 +623,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4CCD827F-1110-48F0-87DC-118EC9F11A1F}" name="Table2" displayName="Table2" ref="A1:G41" insertRowShift="1" totalsRowShown="0" headerRowDxfId="0" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4CCD827F-1110-48F0-87DC-118EC9F11A1F}" name="Table2" displayName="Table2" ref="A1:G41" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9F47A1B3-6180-4DBE-A78C-C596E4AFB4D0}" name="TestID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{7F9DECD0-6444-4DD7-A3D6-EE92ECBA6C1B}" name="TestTitle" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{1102ECA5-FC26-4083-A249-1FFEC0E597C1}" name="Details/Inputs/Actions" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{90CB21A7-7F4A-429B-B6F5-E8CCE53F52EA}" name="Expected Outcome" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{39E1374C-EE38-470E-8AD6-0ED2A590CFDB}" name="Actual Outcome" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{583F42EF-8AA2-4222-A9AE-ABCCA0A16D8A}" name="Result" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{1BAA93F4-E212-42AA-B82C-D21C29A9BDFE}" name="Comment" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9F47A1B3-6180-4DBE-A78C-C596E4AFB4D0}" name="TestID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7F9DECD0-6444-4DD7-A3D6-EE92ECBA6C1B}" name="TestTitle" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1102ECA5-FC26-4083-A249-1FFEC0E597C1}" name="Details/Inputs/Actions" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{90CB21A7-7F4A-429B-B6F5-E8CCE53F52EA}" name="Expected Outcome" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{39E1374C-EE38-470E-8AD6-0ED2A590CFDB}" name="Actual Outcome" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{583F42EF-8AA2-4222-A9AE-ABCCA0A16D8A}" name="Result" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1BAA93F4-E212-42AA-B82C-D21C29A9BDFE}" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -951,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131753A6-1BBD-4EB3-9A13-C3B78D57DD4C}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -993,9 +978,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1006,9 +989,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1019,9 +1000,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1032,9 +1011,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1045,9 +1022,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1451,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122297D2-164C-4A5B-9FCD-5E7326A91898}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>